<commit_message>
changed booklets to real documented files
</commit_message>
<xml_diff>
--- a/booklets/booklets/cocomo_computing.xlsx
+++ b/booklets/booklets/cocomo_computing.xlsx
@@ -207,8 +207,7 @@
   </si>
   <si>
     <t xml:space="preserve">we think we have a good consistency of 
-Our objectives but we are not always
- On the same line</t>
+Our objectives</t>
   </si>
   <si>
     <t xml:space="preserve">Ability, willingness of
@@ -225,8 +224,7 @@
 operating as a team </t>
   </si>
   <si>
-    <t xml:space="preserve">we know each other since 3 years but we
-Didn’t have many times to work as a team</t>
+    <t xml:space="preserve">we know each other since 3 years</t>
   </si>
   <si>
     <t xml:space="preserve">Stakeholder teambuilding to
@@ -235,8 +233,7 @@
   </si>
   <si>
     <t xml:space="preserve">we are friends and we use to hang out
-Some times but it is not this much as
-A teambuilding</t>
+Some times we think this can count as teambuilding since it makes our union stronger</t>
   </si>
   <si>
     <t xml:space="preserve">PMAT</t>
@@ -267,7 +264,7 @@
   <si>
     <t xml:space="preserve">our database grows up pretty fast since we 
 are managing both chat and attachments, 
-we extimated D/P = ~1600 using FP 
+we extimated D/P = ~43 using FP 
 converting to java SLOC And dividing 
 the expected size of the Database with 
 The resulting value </t>
@@ -440,6 +437,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -461,6 +459,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -511,12 +510,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -528,7 +535,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -549,13 +556,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:J1123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C60" activeCellId="0" sqref="C60"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.31"/>
@@ -583,16 +590,16 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="str">
+      <c r="D2" s="3" t="str">
         <f aca="false">INDEX($I$3:$I$8, MATCH(ROUNDDOWN(F2, 0), $J$3:$J$8, 0))</f>
         <v>nominal</v>
       </c>
@@ -608,13 +615,13 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="0" t="str">
+      <c r="D3" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F3, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
@@ -633,13 +640,13 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="str">
+      <c r="D4" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F4, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
@@ -658,17 +665,17 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="0" t="str">
+      <c r="D5" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F5, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="0" t="n">
@@ -683,17 +690,17 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="0" t="str">
+      <c r="D6" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F6, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F6" s="0" t="n">
@@ -711,7 +718,7 @@
       <c r="A7" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="0" t="str">
+      <c r="D7" s="3" t="str">
         <f aca="false">INDEX($I$3:$I$8, MATCH(ROUNDDOWN(F7, 0), $J$3:$J$8, 0))</f>
         <v>high</v>
       </c>
@@ -727,17 +734,17 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="0" t="str">
+      <c r="D8" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F8, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="0" t="n">
@@ -752,13 +759,13 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="0" t="str">
+      <c r="D9" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F9, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
@@ -771,17 +778,17 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="0" t="str">
+      <c r="D10" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F10, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="4" t="s">
         <v>29</v>
       </c>
       <c r="F10" s="0" t="n">
@@ -793,7 +800,7 @@
       <c r="A11" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="0" t="str">
+      <c r="D11" s="3" t="str">
         <f aca="false">INDEX($I$3:$I$8, MATCH(ROUNDDOWN(F11, 0), $J$3:$J$8, 0))</f>
         <v>low</v>
       </c>
@@ -803,17 +810,17 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="0" t="str">
+      <c r="D12" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F12, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="4" t="s">
         <v>32</v>
       </c>
       <c r="F12" s="0" t="n">
@@ -822,17 +829,17 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="0" t="str">
+      <c r="D13" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F13, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="4" t="s">
         <v>34</v>
       </c>
       <c r="F13" s="0" t="n">
@@ -841,17 +848,17 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="0" t="str">
+      <c r="D14" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F14, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="4" t="s">
         <v>36</v>
       </c>
       <c r="F14" s="0" t="n">
@@ -860,17 +867,17 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="0" t="str">
+      <c r="D15" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F15, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="4" t="s">
         <v>38</v>
       </c>
       <c r="F15" s="0" t="n">
@@ -879,17 +886,17 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="0" t="str">
+      <c r="D16" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F16, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="4" t="s">
         <v>40</v>
       </c>
       <c r="F16" s="0" t="n">
@@ -898,17 +905,17 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="0" t="str">
+      <c r="D17" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F17, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F17" s="0" t="n">
@@ -917,17 +924,17 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>43</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="0" t="str">
+      <c r="D18" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F18, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="4" t="s">
         <v>44</v>
       </c>
       <c r="F18" s="0" t="n">
@@ -939,46 +946,46 @@
       <c r="A19" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="0" t="str">
+      <c r="D19" s="3" t="str">
         <f aca="false">INDEX($I$3:$I$8, MATCH(ROUNDDOWN(F19, 0), $J$3:$J$8, 0))</f>
-        <v>nominal</v>
+        <v>high</v>
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">SUM(F20:F23)/4</f>
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D20" s="0" t="str">
+        <v>16</v>
+      </c>
+      <c r="D20" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F20, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="4" t="s">
         <v>47</v>
       </c>
       <c r="F20" s="0" t="n">
         <f aca="false">VLOOKUP(C20, $I$3:$J$8, 2, 0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="0" t="str">
+      <c r="D21" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F21, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="4" t="s">
         <v>49</v>
       </c>
       <c r="F21" s="0" t="n">
@@ -987,48 +994,48 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="0" t="str">
+        <v>16</v>
+      </c>
+      <c r="D22" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F22, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="4" t="s">
         <v>51</v>
       </c>
       <c r="F22" s="0" t="n">
         <f aca="false">VLOOKUP(C22, $I$3:$J$8, 2, 0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="0" t="str">
+        <v>16</v>
+      </c>
+      <c r="D23" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F23, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="4" t="s">
         <v>53</v>
       </c>
       <c r="F23" s="0" t="n">
         <f aca="false">VLOOKUP(C23, $I$3:$J$8, 2, 0)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="D24" s="0" t="str">
+      <c r="D24" s="3" t="str">
         <f aca="false">C25</f>
         <v>low</v>
       </c>
@@ -1044,7 +1051,7 @@
       <c r="C25" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="0" t="str">
+      <c r="D25" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F25, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
@@ -1057,15 +1064,15 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4" t="str">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F26, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3" t="e">
+      <c r="E26" s="5"/>
+      <c r="F26" s="5" t="e">
         <f aca="false">VLOOKUP(C26, $I$3:$J$8, 2, 0)</f>
         <v>#N/A</v>
       </c>
@@ -1074,7 +1081,7 @@
       <c r="A27" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D27" s="0" t="str">
+      <c r="D27" s="3" t="str">
         <f aca="false">C28</f>
         <v>low</v>
       </c>
@@ -1090,11 +1097,11 @@
       <c r="C28" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="0" t="str">
+      <c r="D28" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F28, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="4" t="s">
         <v>59</v>
       </c>
       <c r="F28" s="0" t="n">
@@ -1106,9 +1113,9 @@
       <c r="A29" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="D29" s="0" t="str">
+      <c r="D29" s="3" t="str">
         <f aca="false">C30</f>
-        <v>very high</v>
+        <v>nominal</v>
       </c>
       <c r="F29" s="0" t="e">
         <f aca="false">VLOOKUP(C29, $I$3:$J$8, 2, 0)</f>
@@ -1120,25 +1127,25 @@
         <v>61</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="D30" s="0" t="str">
+        <v>18</v>
+      </c>
+      <c r="D30" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F30, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="4" t="s">
         <v>62</v>
       </c>
       <c r="F30" s="0" t="n">
         <f aca="false">VLOOKUP(C30, $I$3:$J$8, 2, 0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="D31" s="0" t="str">
+      <c r="D31" s="3" t="str">
         <f aca="false">INDEX($I$3:$I$8, MATCH(ROUNDDOWN(F31, 0), $J$3:$J$8, 0))</f>
         <v>low</v>
       </c>
@@ -1154,11 +1161,11 @@
       <c r="C32" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="0" t="str">
+      <c r="D32" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F32, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="4" t="s">
         <v>65</v>
       </c>
       <c r="F32" s="0" t="n">
@@ -1173,11 +1180,11 @@
       <c r="C33" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="0" t="str">
+      <c r="D33" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F33, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="4" t="s">
         <v>67</v>
       </c>
       <c r="F33" s="0" t="n">
@@ -1192,11 +1199,11 @@
       <c r="C34" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="0" t="str">
+      <c r="D34" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F34, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="4" t="s">
         <v>69</v>
       </c>
       <c r="F34" s="0" t="n">
@@ -1211,11 +1218,11 @@
       <c r="C35" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="0" t="str">
+      <c r="D35" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F35, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="4" t="s">
         <v>71</v>
       </c>
       <c r="F35" s="0" t="n">
@@ -1230,11 +1237,11 @@
       <c r="C36" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="0" t="str">
+      <c r="D36" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F36, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="4" t="s">
         <v>73</v>
       </c>
       <c r="F36" s="0" t="n">
@@ -1246,7 +1253,7 @@
       <c r="A37" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="D37" s="0" t="str">
+      <c r="D37" s="3" t="str">
         <f aca="false">C38</f>
         <v>low</v>
       </c>
@@ -1262,7 +1269,7 @@
       <c r="C38" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="0" t="str">
+      <c r="D38" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F38, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
@@ -1278,7 +1285,7 @@
       <c r="A39" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="D39" s="0" t="str">
+      <c r="D39" s="3" t="str">
         <f aca="false">C40</f>
         <v>low</v>
       </c>
@@ -1294,7 +1301,8 @@
       <c r="C40" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="D40" s="3"/>
+      <c r="E40" s="4" t="s">
         <v>77</v>
       </c>
       <c r="F40" s="0" t="n">
@@ -1306,7 +1314,7 @@
       <c r="A41" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="0" t="str">
+      <c r="D41" s="3" t="str">
         <f aca="false">C42</f>
         <v>nominal</v>
       </c>
@@ -1322,7 +1330,8 @@
       <c r="C42" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E42" s="2" t="s">
+      <c r="D42" s="3"/>
+      <c r="E42" s="4" t="s">
         <v>79</v>
       </c>
       <c r="F42" s="0" t="n">
@@ -1334,7 +1343,7 @@
       <c r="A43" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="D43" s="0" t="str">
+      <c r="D43" s="3" t="str">
         <f aca="false">C44</f>
         <v>nominal</v>
       </c>
@@ -1350,7 +1359,8 @@
       <c r="C44" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="D44" s="3"/>
+      <c r="E44" s="4" t="s">
         <v>81</v>
       </c>
       <c r="F44" s="0" t="n">
@@ -1362,7 +1372,7 @@
       <c r="A45" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="D45" s="0" t="str">
+      <c r="D45" s="3" t="str">
         <f aca="false">C46</f>
         <v>low</v>
       </c>
@@ -1378,7 +1388,8 @@
       <c r="C46" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="D46" s="3"/>
+      <c r="E46" s="4" t="s">
         <v>83</v>
       </c>
       <c r="F46" s="0" t="n">
@@ -1390,7 +1401,7 @@
       <c r="A47" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="D47" s="0" t="str">
+      <c r="D47" s="3" t="str">
         <f aca="false">C48</f>
         <v>low</v>
       </c>
@@ -1406,7 +1417,8 @@
       <c r="C48" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="D48" s="3"/>
+      <c r="E48" s="4" t="s">
         <v>85</v>
       </c>
       <c r="F48" s="0" t="n">
@@ -1418,7 +1430,7 @@
       <c r="A49" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="D49" s="0" t="str">
+      <c r="D49" s="3" t="str">
         <f aca="false">C50</f>
         <v>low</v>
       </c>
@@ -1434,7 +1446,8 @@
       <c r="C50" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="D50" s="3"/>
+      <c r="E50" s="4" t="s">
         <v>87</v>
       </c>
       <c r="F50" s="0" t="n">
@@ -1446,7 +1459,7 @@
       <c r="A51" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="D51" s="0" t="str">
+      <c r="D51" s="3" t="str">
         <f aca="false">C52</f>
         <v>very high</v>
       </c>
@@ -1462,7 +1475,8 @@
       <c r="C52" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="E52" s="2" t="s">
+      <c r="D52" s="3"/>
+      <c r="E52" s="4" t="s">
         <v>89</v>
       </c>
       <c r="F52" s="0" t="n">
@@ -1474,7 +1488,7 @@
       <c r="A53" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D53" s="0" t="str">
+      <c r="D53" s="3" t="str">
         <f aca="false">C54</f>
         <v>very low</v>
       </c>
@@ -1490,7 +1504,8 @@
       <c r="C54" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E54" s="2" t="s">
+      <c r="D54" s="3"/>
+      <c r="E54" s="4" t="s">
         <v>91</v>
       </c>
       <c r="F54" s="0" t="n">
@@ -1502,7 +1517,7 @@
       <c r="A55" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="D55" s="0" t="str">
+      <c r="D55" s="3" t="str">
         <f aca="false">C56</f>
         <v>very low</v>
       </c>
@@ -1518,7 +1533,8 @@
       <c r="C56" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="E56" s="2" t="s">
+      <c r="D56" s="3"/>
+      <c r="E56" s="4" t="s">
         <v>93</v>
       </c>
       <c r="F56" s="0" t="n">
@@ -1530,7 +1546,7 @@
       <c r="A57" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="D57" s="0" t="str">
+      <c r="D57" s="3" t="str">
         <f aca="false">C58</f>
         <v>nominal</v>
       </c>
@@ -1546,7 +1562,8 @@
       <c r="C58" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="D58" s="3"/>
+      <c r="E58" s="4" t="s">
         <v>95</v>
       </c>
       <c r="F58" s="0" t="n">
@@ -1558,7 +1575,7 @@
       <c r="A59" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="D59" s="0" t="str">
+      <c r="D59" s="3" t="str">
         <f aca="false">C60</f>
         <v>nominal</v>
       </c>
@@ -1574,7 +1591,8 @@
       <c r="C60" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E60" s="2" t="s">
+      <c r="D60" s="3"/>
+      <c r="E60" s="4" t="s">
         <v>97</v>
       </c>
       <c r="F60" s="0" t="n">
@@ -1586,7 +1604,7 @@
       <c r="A61" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="D61" s="0" t="str">
+      <c r="D61" s="3" t="str">
         <f aca="false">INDEX($I$3:$I$8, MATCH(ROUNDDOWN(F61, 0), $J$3:$J$8, 0))</f>
         <v>nominal</v>
       </c>
@@ -1602,11 +1620,11 @@
       <c r="C62" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D62" s="0" t="str">
+      <c r="D62" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F62, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
-      <c r="E62" s="2" t="s">
+      <c r="E62" s="4" t="s">
         <v>100</v>
       </c>
       <c r="F62" s="0" t="n">
@@ -1621,7 +1639,7 @@
       <c r="C63" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D63" s="0" t="str">
+      <c r="D63" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F63, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
@@ -1637,7 +1655,7 @@
       <c r="A64" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="D64" s="0" t="str">
+      <c r="D64" s="3" t="str">
         <f aca="false">C65</f>
         <v>nominal</v>
       </c>
@@ -1653,7 +1671,7 @@
       <c r="C65" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D65" s="0" t="str">
+      <c r="D65" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F65, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
@@ -1666,352 +1684,3352 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D66" s="0" t="str">
+      <c r="D66" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F66, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D67" s="0" t="str">
+      <c r="D67" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F67, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="0" t="str">
+      <c r="D68" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F68, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D69" s="0" t="str">
+      <c r="D69" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F69, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D70" s="0" t="str">
+      <c r="D70" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F70, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D71" s="0" t="str">
+      <c r="D71" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F71, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D72" s="0" t="str">
+      <c r="D72" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F72, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D73" s="0" t="str">
+      <c r="D73" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F73, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D74" s="0" t="str">
+      <c r="D74" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F74, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D75" s="0" t="str">
+      <c r="D75" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F75, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D76" s="0" t="str">
+      <c r="D76" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F76, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D77" s="0" t="str">
+      <c r="D77" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F77, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D78" s="0" t="str">
+      <c r="D78" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F78, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D79" s="0" t="str">
+      <c r="D79" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F79, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D80" s="0" t="str">
+      <c r="D80" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F80, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D81" s="0" t="str">
+      <c r="D81" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F81, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D82" s="0" t="str">
+      <c r="D82" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F82, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D83" s="0" t="str">
+      <c r="D83" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F83, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D84" s="0" t="str">
+      <c r="D84" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F84, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D85" s="0" t="str">
+      <c r="D85" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F85, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D86" s="0" t="str">
+      <c r="D86" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F86, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D87" s="0" t="str">
+      <c r="D87" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F87, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D88" s="0" t="str">
+      <c r="D88" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F88, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D89" s="0" t="str">
+      <c r="D89" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F89, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D90" s="0" t="str">
+      <c r="D90" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F90, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D91" s="0" t="str">
+      <c r="D91" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F91, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D92" s="0" t="str">
+      <c r="D92" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F92, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D93" s="0" t="str">
+      <c r="D93" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F93, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D94" s="0" t="str">
+      <c r="D94" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F94, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D95" s="0" t="str">
+      <c r="D95" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F95, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D96" s="0" t="str">
+      <c r="D96" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F96, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D97" s="0" t="str">
+      <c r="D97" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F97, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D98" s="0" t="str">
+      <c r="D98" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F98, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D99" s="0" t="str">
+      <c r="D99" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F99, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D100" s="0" t="str">
+      <c r="D100" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F100, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D101" s="0" t="str">
+      <c r="D101" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F101, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D102" s="0" t="str">
+      <c r="D102" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F102, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D103" s="0" t="str">
+      <c r="D103" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F103, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D104" s="0" t="str">
+      <c r="D104" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F104, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D105" s="0" t="str">
+      <c r="D105" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F105, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D106" s="0" t="str">
+      <c r="D106" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F106, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D107" s="0" t="str">
+      <c r="D107" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F107, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D108" s="0" t="str">
+      <c r="D108" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F108, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D109" s="0" t="str">
+      <c r="D109" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F109, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D110" s="0" t="str">
+      <c r="D110" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F110, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D111" s="0" t="str">
+      <c r="D111" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F111, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D112" s="0" t="str">
+      <c r="D112" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F112, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D113" s="0" t="str">
+      <c r="D113" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F113, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D114" s="0" t="str">
+      <c r="D114" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F114, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D115" s="0" t="str">
+      <c r="D115" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F115, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D116" s="0" t="str">
+      <c r="D116" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F116, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D117" s="0" t="str">
+      <c r="D117" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F117, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D118" s="0" t="str">
+      <c r="D118" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F118, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D119" s="0" t="str">
+      <c r="D119" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F119, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D120" s="0" t="str">
+      <c r="D120" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F120, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D121" s="0" t="str">
+      <c r="D121" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F121, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D122" s="0" t="str">
+      <c r="D122" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F122, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D123" s="0" t="str">
+      <c r="D123" s="3" t="str">
         <f aca="false">IFERROR(VLOOKUP(ROUNDDOWN(F123, 1), $I$3:$J$8, 2, 1), "")</f>
         <v/>
       </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D124" s="3"/>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D125" s="3"/>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D126" s="3"/>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D127" s="3"/>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D128" s="3"/>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D129" s="3"/>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D130" s="3"/>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D131" s="3"/>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D132" s="3"/>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D133" s="3"/>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D134" s="3"/>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D135" s="3"/>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D136" s="3"/>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D137" s="3"/>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D138" s="3"/>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D139" s="3"/>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D140" s="3"/>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D141" s="3"/>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D142" s="3"/>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D143" s="3"/>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D144" s="3"/>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D145" s="3"/>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D146" s="3"/>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D147" s="3"/>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D148" s="3"/>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D149" s="3"/>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D150" s="3"/>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D151" s="3"/>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D152" s="3"/>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D153" s="3"/>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D154" s="3"/>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D155" s="3"/>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D156" s="3"/>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D157" s="3"/>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D158" s="3"/>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D159" s="3"/>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D160" s="3"/>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D161" s="3"/>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D162" s="3"/>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D163" s="3"/>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D164" s="3"/>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D165" s="3"/>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D166" s="3"/>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D167" s="3"/>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D168" s="3"/>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D169" s="3"/>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D170" s="3"/>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D171" s="3"/>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D172" s="3"/>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D173" s="3"/>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D174" s="3"/>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D175" s="3"/>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D176" s="3"/>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D177" s="3"/>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D178" s="3"/>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D179" s="3"/>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D180" s="3"/>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D181" s="3"/>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D182" s="3"/>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D183" s="3"/>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D184" s="3"/>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D185" s="3"/>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D186" s="3"/>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D187" s="3"/>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D188" s="3"/>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D189" s="3"/>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D190" s="3"/>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D191" s="3"/>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D192" s="3"/>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D193" s="3"/>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D194" s="3"/>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D195" s="3"/>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D196" s="3"/>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D197" s="3"/>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D198" s="3"/>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D199" s="3"/>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D200" s="3"/>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D201" s="3"/>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D202" s="3"/>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D203" s="3"/>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D204" s="3"/>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D205" s="3"/>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D206" s="3"/>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D207" s="3"/>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D208" s="3"/>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D209" s="3"/>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D210" s="3"/>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D211" s="3"/>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D212" s="3"/>
+    </row>
+    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D213" s="3"/>
+    </row>
+    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D214" s="3"/>
+    </row>
+    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D215" s="3"/>
+    </row>
+    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D216" s="3"/>
+    </row>
+    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D217" s="3"/>
+    </row>
+    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D218" s="3"/>
+    </row>
+    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D219" s="3"/>
+    </row>
+    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D220" s="3"/>
+    </row>
+    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D221" s="3"/>
+    </row>
+    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D222" s="3"/>
+    </row>
+    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D223" s="3"/>
+    </row>
+    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D224" s="3"/>
+    </row>
+    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D225" s="3"/>
+    </row>
+    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D226" s="3"/>
+    </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D227" s="3"/>
+    </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D228" s="3"/>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D229" s="3"/>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D230" s="3"/>
+    </row>
+    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D231" s="3"/>
+    </row>
+    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D232" s="3"/>
+    </row>
+    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D233" s="3"/>
+    </row>
+    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D234" s="3"/>
+    </row>
+    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D235" s="3"/>
+    </row>
+    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D236" s="3"/>
+    </row>
+    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D237" s="3"/>
+    </row>
+    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D238" s="3"/>
+    </row>
+    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D239" s="3"/>
+    </row>
+    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D240" s="3"/>
+    </row>
+    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D241" s="3"/>
+    </row>
+    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D242" s="3"/>
+    </row>
+    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D243" s="3"/>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D244" s="3"/>
+    </row>
+    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D245" s="3"/>
+    </row>
+    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D246" s="3"/>
+    </row>
+    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D247" s="3"/>
+    </row>
+    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D248" s="3"/>
+    </row>
+    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D249" s="3"/>
+    </row>
+    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D250" s="3"/>
+    </row>
+    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D251" s="3"/>
+    </row>
+    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D252" s="3"/>
+    </row>
+    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D253" s="3"/>
+    </row>
+    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D254" s="3"/>
+    </row>
+    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D255" s="3"/>
+    </row>
+    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D256" s="3"/>
+    </row>
+    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D257" s="3"/>
+    </row>
+    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D258" s="3"/>
+    </row>
+    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D259" s="3"/>
+    </row>
+    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D260" s="3"/>
+    </row>
+    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D261" s="3"/>
+    </row>
+    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D262" s="3"/>
+    </row>
+    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D263" s="3"/>
+    </row>
+    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D264" s="3"/>
+    </row>
+    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D265" s="3"/>
+    </row>
+    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D266" s="3"/>
+    </row>
+    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D267" s="3"/>
+    </row>
+    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D268" s="3"/>
+    </row>
+    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D269" s="3"/>
+    </row>
+    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D270" s="3"/>
+    </row>
+    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D271" s="3"/>
+    </row>
+    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D272" s="3"/>
+    </row>
+    <row r="273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D273" s="3"/>
+    </row>
+    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D274" s="3"/>
+    </row>
+    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D275" s="3"/>
+    </row>
+    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D276" s="3"/>
+    </row>
+    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D277" s="3"/>
+    </row>
+    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D278" s="3"/>
+    </row>
+    <row r="279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D279" s="3"/>
+    </row>
+    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D280" s="3"/>
+    </row>
+    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D281" s="3"/>
+    </row>
+    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D282" s="3"/>
+    </row>
+    <row r="283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D283" s="3"/>
+    </row>
+    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D284" s="3"/>
+    </row>
+    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D285" s="3"/>
+    </row>
+    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D286" s="3"/>
+    </row>
+    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D287" s="3"/>
+    </row>
+    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D288" s="3"/>
+    </row>
+    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D289" s="3"/>
+    </row>
+    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D290" s="3"/>
+    </row>
+    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D291" s="3"/>
+    </row>
+    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D292" s="3"/>
+    </row>
+    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D293" s="3"/>
+    </row>
+    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D294" s="3"/>
+    </row>
+    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D295" s="3"/>
+    </row>
+    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D296" s="3"/>
+    </row>
+    <row r="297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D297" s="3"/>
+    </row>
+    <row r="298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D298" s="3"/>
+    </row>
+    <row r="299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D299" s="3"/>
+    </row>
+    <row r="300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D300" s="3"/>
+    </row>
+    <row r="301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D301" s="3"/>
+    </row>
+    <row r="302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D302" s="3"/>
+    </row>
+    <row r="303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D303" s="3"/>
+    </row>
+    <row r="304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D304" s="3"/>
+    </row>
+    <row r="305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D305" s="3"/>
+    </row>
+    <row r="306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D306" s="3"/>
+    </row>
+    <row r="307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D307" s="3"/>
+    </row>
+    <row r="308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D308" s="3"/>
+    </row>
+    <row r="309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D309" s="3"/>
+    </row>
+    <row r="310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D310" s="3"/>
+    </row>
+    <row r="311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D311" s="3"/>
+    </row>
+    <row r="312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D312" s="3"/>
+    </row>
+    <row r="313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D313" s="3"/>
+    </row>
+    <row r="314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D314" s="3"/>
+    </row>
+    <row r="315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D315" s="3"/>
+    </row>
+    <row r="316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D316" s="3"/>
+    </row>
+    <row r="317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D317" s="3"/>
+    </row>
+    <row r="318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D318" s="3"/>
+    </row>
+    <row r="319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D319" s="3"/>
+    </row>
+    <row r="320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D320" s="3"/>
+    </row>
+    <row r="321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D321" s="3"/>
+    </row>
+    <row r="322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D322" s="3"/>
+    </row>
+    <row r="323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D323" s="3"/>
+    </row>
+    <row r="324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D324" s="3"/>
+    </row>
+    <row r="325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D325" s="3"/>
+    </row>
+    <row r="326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D326" s="3"/>
+    </row>
+    <row r="327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D327" s="3"/>
+    </row>
+    <row r="328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D328" s="3"/>
+    </row>
+    <row r="329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D329" s="3"/>
+    </row>
+    <row r="330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D330" s="3"/>
+    </row>
+    <row r="331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D331" s="3"/>
+    </row>
+    <row r="332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D332" s="3"/>
+    </row>
+    <row r="333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D333" s="3"/>
+    </row>
+    <row r="334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D334" s="3"/>
+    </row>
+    <row r="335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D335" s="3"/>
+    </row>
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D336" s="3"/>
+    </row>
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D337" s="3"/>
+    </row>
+    <row r="338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D338" s="3"/>
+    </row>
+    <row r="339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D339" s="3"/>
+    </row>
+    <row r="340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D340" s="3"/>
+    </row>
+    <row r="341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D341" s="3"/>
+    </row>
+    <row r="342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D342" s="3"/>
+    </row>
+    <row r="343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D343" s="3"/>
+    </row>
+    <row r="344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D344" s="3"/>
+    </row>
+    <row r="345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D345" s="3"/>
+    </row>
+    <row r="346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D346" s="3"/>
+    </row>
+    <row r="347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D347" s="3"/>
+    </row>
+    <row r="348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D348" s="3"/>
+    </row>
+    <row r="349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D349" s="3"/>
+    </row>
+    <row r="350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D350" s="3"/>
+    </row>
+    <row r="351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D351" s="3"/>
+    </row>
+    <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D352" s="3"/>
+    </row>
+    <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D353" s="3"/>
+    </row>
+    <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D354" s="3"/>
+    </row>
+    <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D355" s="3"/>
+    </row>
+    <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D356" s="3"/>
+    </row>
+    <row r="357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D357" s="3"/>
+    </row>
+    <row r="358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D358" s="3"/>
+    </row>
+    <row r="359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D359" s="3"/>
+    </row>
+    <row r="360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D360" s="3"/>
+    </row>
+    <row r="361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D361" s="3"/>
+    </row>
+    <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D362" s="3"/>
+    </row>
+    <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D363" s="3"/>
+    </row>
+    <row r="364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D364" s="3"/>
+    </row>
+    <row r="365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D365" s="3"/>
+    </row>
+    <row r="366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D366" s="3"/>
+    </row>
+    <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D367" s="3"/>
+    </row>
+    <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D368" s="3"/>
+    </row>
+    <row r="369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D369" s="3"/>
+    </row>
+    <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D370" s="3"/>
+    </row>
+    <row r="371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D371" s="3"/>
+    </row>
+    <row r="372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D372" s="3"/>
+    </row>
+    <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D373" s="3"/>
+    </row>
+    <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D374" s="3"/>
+    </row>
+    <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D375" s="3"/>
+    </row>
+    <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D376" s="3"/>
+    </row>
+    <row r="377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D377" s="3"/>
+    </row>
+    <row r="378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D378" s="3"/>
+    </row>
+    <row r="379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D379" s="3"/>
+    </row>
+    <row r="380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D380" s="3"/>
+    </row>
+    <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D381" s="3"/>
+    </row>
+    <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D382" s="3"/>
+    </row>
+    <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D383" s="3"/>
+    </row>
+    <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D384" s="3"/>
+    </row>
+    <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D385" s="3"/>
+    </row>
+    <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D386" s="3"/>
+    </row>
+    <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D387" s="3"/>
+    </row>
+    <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D388" s="3"/>
+    </row>
+    <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D389" s="3"/>
+    </row>
+    <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D390" s="3"/>
+    </row>
+    <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D391" s="3"/>
+    </row>
+    <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D392" s="3"/>
+    </row>
+    <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D393" s="3"/>
+    </row>
+    <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D394" s="3"/>
+    </row>
+    <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D395" s="3"/>
+    </row>
+    <row r="396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D396" s="3"/>
+    </row>
+    <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D397" s="3"/>
+    </row>
+    <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D398" s="3"/>
+    </row>
+    <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D399" s="3"/>
+    </row>
+    <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D400" s="3"/>
+    </row>
+    <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D401" s="3"/>
+    </row>
+    <row r="402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D402" s="3"/>
+    </row>
+    <row r="403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D403" s="3"/>
+    </row>
+    <row r="404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D404" s="3"/>
+    </row>
+    <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D405" s="3"/>
+    </row>
+    <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D406" s="3"/>
+    </row>
+    <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D407" s="3"/>
+    </row>
+    <row r="408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D408" s="3"/>
+    </row>
+    <row r="409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D409" s="3"/>
+    </row>
+    <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D410" s="3"/>
+    </row>
+    <row r="411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D411" s="3"/>
+    </row>
+    <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D412" s="3"/>
+    </row>
+    <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D413" s="3"/>
+    </row>
+    <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D414" s="3"/>
+    </row>
+    <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D415" s="3"/>
+    </row>
+    <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D416" s="3"/>
+    </row>
+    <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D417" s="3"/>
+    </row>
+    <row r="418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D418" s="3"/>
+    </row>
+    <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D419" s="3"/>
+    </row>
+    <row r="420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D420" s="3"/>
+    </row>
+    <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D421" s="3"/>
+    </row>
+    <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D422" s="3"/>
+    </row>
+    <row r="423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D423" s="3"/>
+    </row>
+    <row r="424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D424" s="3"/>
+    </row>
+    <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D425" s="3"/>
+    </row>
+    <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D426" s="3"/>
+    </row>
+    <row r="427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D427" s="3"/>
+    </row>
+    <row r="428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D428" s="3"/>
+    </row>
+    <row r="429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D429" s="3"/>
+    </row>
+    <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D430" s="3"/>
+    </row>
+    <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D431" s="3"/>
+    </row>
+    <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D432" s="3"/>
+    </row>
+    <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D433" s="3"/>
+    </row>
+    <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D434" s="3"/>
+    </row>
+    <row r="435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D435" s="3"/>
+    </row>
+    <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D436" s="3"/>
+    </row>
+    <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D437" s="3"/>
+    </row>
+    <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D438" s="3"/>
+    </row>
+    <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D439" s="3"/>
+    </row>
+    <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D440" s="3"/>
+    </row>
+    <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D441" s="3"/>
+    </row>
+    <row r="442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D442" s="3"/>
+    </row>
+    <row r="443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D443" s="3"/>
+    </row>
+    <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D444" s="3"/>
+    </row>
+    <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D445" s="3"/>
+    </row>
+    <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D446" s="3"/>
+    </row>
+    <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D447" s="3"/>
+    </row>
+    <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D448" s="3"/>
+    </row>
+    <row r="449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D449" s="3"/>
+    </row>
+    <row r="450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D450" s="3"/>
+    </row>
+    <row r="451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D451" s="3"/>
+    </row>
+    <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D452" s="3"/>
+    </row>
+    <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D453" s="3"/>
+    </row>
+    <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D454" s="3"/>
+    </row>
+    <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D455" s="3"/>
+    </row>
+    <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D456" s="3"/>
+    </row>
+    <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D457" s="3"/>
+    </row>
+    <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D458" s="3"/>
+    </row>
+    <row r="459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D459" s="3"/>
+    </row>
+    <row r="460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D460" s="3"/>
+    </row>
+    <row r="461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D461" s="3"/>
+    </row>
+    <row r="462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D462" s="3"/>
+    </row>
+    <row r="463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D463" s="3"/>
+    </row>
+    <row r="464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D464" s="3"/>
+    </row>
+    <row r="465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D465" s="3"/>
+    </row>
+    <row r="466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D466" s="3"/>
+    </row>
+    <row r="467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D467" s="3"/>
+    </row>
+    <row r="468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D468" s="3"/>
+    </row>
+    <row r="469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D469" s="3"/>
+    </row>
+    <row r="470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D470" s="3"/>
+    </row>
+    <row r="471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D471" s="3"/>
+    </row>
+    <row r="472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D472" s="3"/>
+    </row>
+    <row r="473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D473" s="3"/>
+    </row>
+    <row r="474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D474" s="3"/>
+    </row>
+    <row r="475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D475" s="3"/>
+    </row>
+    <row r="476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D476" s="3"/>
+    </row>
+    <row r="477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D477" s="3"/>
+    </row>
+    <row r="478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D478" s="3"/>
+    </row>
+    <row r="479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D479" s="3"/>
+    </row>
+    <row r="480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D480" s="3"/>
+    </row>
+    <row r="481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D481" s="3"/>
+    </row>
+    <row r="482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D482" s="3"/>
+    </row>
+    <row r="483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D483" s="3"/>
+    </row>
+    <row r="484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D484" s="3"/>
+    </row>
+    <row r="485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D485" s="3"/>
+    </row>
+    <row r="486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D486" s="3"/>
+    </row>
+    <row r="487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D487" s="3"/>
+    </row>
+    <row r="488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D488" s="3"/>
+    </row>
+    <row r="489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D489" s="3"/>
+    </row>
+    <row r="490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D490" s="3"/>
+    </row>
+    <row r="491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D491" s="3"/>
+    </row>
+    <row r="492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D492" s="3"/>
+    </row>
+    <row r="493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D493" s="3"/>
+    </row>
+    <row r="494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D494" s="3"/>
+    </row>
+    <row r="495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D495" s="3"/>
+    </row>
+    <row r="496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D496" s="3"/>
+    </row>
+    <row r="497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D497" s="3"/>
+    </row>
+    <row r="498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D498" s="3"/>
+    </row>
+    <row r="499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D499" s="3"/>
+    </row>
+    <row r="500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D500" s="3"/>
+    </row>
+    <row r="501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D501" s="3"/>
+    </row>
+    <row r="502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D502" s="3"/>
+    </row>
+    <row r="503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D503" s="3"/>
+    </row>
+    <row r="504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D504" s="3"/>
+    </row>
+    <row r="505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D505" s="3"/>
+    </row>
+    <row r="506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D506" s="3"/>
+    </row>
+    <row r="507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D507" s="3"/>
+    </row>
+    <row r="508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D508" s="3"/>
+    </row>
+    <row r="509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D509" s="3"/>
+    </row>
+    <row r="510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D510" s="3"/>
+    </row>
+    <row r="511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D511" s="3"/>
+    </row>
+    <row r="512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D512" s="3"/>
+    </row>
+    <row r="513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D513" s="3"/>
+    </row>
+    <row r="514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D514" s="3"/>
+    </row>
+    <row r="515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D515" s="3"/>
+    </row>
+    <row r="516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D516" s="3"/>
+    </row>
+    <row r="517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D517" s="3"/>
+    </row>
+    <row r="518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D518" s="3"/>
+    </row>
+    <row r="519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D519" s="3"/>
+    </row>
+    <row r="520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D520" s="3"/>
+    </row>
+    <row r="521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D521" s="3"/>
+    </row>
+    <row r="522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D522" s="3"/>
+    </row>
+    <row r="523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D523" s="3"/>
+    </row>
+    <row r="524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D524" s="3"/>
+    </row>
+    <row r="525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D525" s="3"/>
+    </row>
+    <row r="526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D526" s="3"/>
+    </row>
+    <row r="527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D527" s="3"/>
+    </row>
+    <row r="528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D528" s="3"/>
+    </row>
+    <row r="529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D529" s="3"/>
+    </row>
+    <row r="530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D530" s="3"/>
+    </row>
+    <row r="531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D531" s="3"/>
+    </row>
+    <row r="532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D532" s="3"/>
+    </row>
+    <row r="533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D533" s="3"/>
+    </row>
+    <row r="534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D534" s="3"/>
+    </row>
+    <row r="535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D535" s="3"/>
+    </row>
+    <row r="536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D536" s="3"/>
+    </row>
+    <row r="537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D537" s="3"/>
+    </row>
+    <row r="538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D538" s="3"/>
+    </row>
+    <row r="539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D539" s="3"/>
+    </row>
+    <row r="540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D540" s="3"/>
+    </row>
+    <row r="541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D541" s="3"/>
+    </row>
+    <row r="542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D542" s="3"/>
+    </row>
+    <row r="543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D543" s="3"/>
+    </row>
+    <row r="544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D544" s="3"/>
+    </row>
+    <row r="545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D545" s="3"/>
+    </row>
+    <row r="546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D546" s="3"/>
+    </row>
+    <row r="547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D547" s="3"/>
+    </row>
+    <row r="548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D548" s="3"/>
+    </row>
+    <row r="549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D549" s="3"/>
+    </row>
+    <row r="550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D550" s="3"/>
+    </row>
+    <row r="551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D551" s="3"/>
+    </row>
+    <row r="552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D552" s="3"/>
+    </row>
+    <row r="553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D553" s="3"/>
+    </row>
+    <row r="554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D554" s="3"/>
+    </row>
+    <row r="555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D555" s="3"/>
+    </row>
+    <row r="556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D556" s="3"/>
+    </row>
+    <row r="557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D557" s="3"/>
+    </row>
+    <row r="558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D558" s="3"/>
+    </row>
+    <row r="559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D559" s="3"/>
+    </row>
+    <row r="560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D560" s="3"/>
+    </row>
+    <row r="561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D561" s="3"/>
+    </row>
+    <row r="562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D562" s="3"/>
+    </row>
+    <row r="563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D563" s="3"/>
+    </row>
+    <row r="564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D564" s="3"/>
+    </row>
+    <row r="565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D565" s="3"/>
+    </row>
+    <row r="566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D566" s="3"/>
+    </row>
+    <row r="567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D567" s="3"/>
+    </row>
+    <row r="568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D568" s="3"/>
+    </row>
+    <row r="569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D569" s="3"/>
+    </row>
+    <row r="570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D570" s="3"/>
+    </row>
+    <row r="571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D571" s="3"/>
+    </row>
+    <row r="572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D572" s="3"/>
+    </row>
+    <row r="573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D573" s="3"/>
+    </row>
+    <row r="574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D574" s="3"/>
+    </row>
+    <row r="575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D575" s="3"/>
+    </row>
+    <row r="576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D576" s="3"/>
+    </row>
+    <row r="577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D577" s="3"/>
+    </row>
+    <row r="578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D578" s="3"/>
+    </row>
+    <row r="579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D579" s="3"/>
+    </row>
+    <row r="580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D580" s="3"/>
+    </row>
+    <row r="581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D581" s="3"/>
+    </row>
+    <row r="582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D582" s="3"/>
+    </row>
+    <row r="583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D583" s="3"/>
+    </row>
+    <row r="584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D584" s="3"/>
+    </row>
+    <row r="585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D585" s="3"/>
+    </row>
+    <row r="586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D586" s="3"/>
+    </row>
+    <row r="587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D587" s="3"/>
+    </row>
+    <row r="588" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D588" s="3"/>
+    </row>
+    <row r="589" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D589" s="3"/>
+    </row>
+    <row r="590" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D590" s="3"/>
+    </row>
+    <row r="591" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D591" s="3"/>
+    </row>
+    <row r="592" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D592" s="3"/>
+    </row>
+    <row r="593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D593" s="3"/>
+    </row>
+    <row r="594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D594" s="3"/>
+    </row>
+    <row r="595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D595" s="3"/>
+    </row>
+    <row r="596" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D596" s="3"/>
+    </row>
+    <row r="597" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D597" s="3"/>
+    </row>
+    <row r="598" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D598" s="3"/>
+    </row>
+    <row r="599" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D599" s="3"/>
+    </row>
+    <row r="600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D600" s="3"/>
+    </row>
+    <row r="601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D601" s="3"/>
+    </row>
+    <row r="602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D602" s="3"/>
+    </row>
+    <row r="603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D603" s="3"/>
+    </row>
+    <row r="604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D604" s="3"/>
+    </row>
+    <row r="605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D605" s="3"/>
+    </row>
+    <row r="606" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D606" s="3"/>
+    </row>
+    <row r="607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D607" s="3"/>
+    </row>
+    <row r="608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D608" s="3"/>
+    </row>
+    <row r="609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D609" s="3"/>
+    </row>
+    <row r="610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D610" s="3"/>
+    </row>
+    <row r="611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D611" s="3"/>
+    </row>
+    <row r="612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D612" s="3"/>
+    </row>
+    <row r="613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D613" s="3"/>
+    </row>
+    <row r="614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D614" s="3"/>
+    </row>
+    <row r="615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D615" s="3"/>
+    </row>
+    <row r="616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D616" s="3"/>
+    </row>
+    <row r="617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D617" s="3"/>
+    </row>
+    <row r="618" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D618" s="3"/>
+    </row>
+    <row r="619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D619" s="3"/>
+    </row>
+    <row r="620" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D620" s="3"/>
+    </row>
+    <row r="621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D621" s="3"/>
+    </row>
+    <row r="622" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D622" s="3"/>
+    </row>
+    <row r="623" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D623" s="3"/>
+    </row>
+    <row r="624" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D624" s="3"/>
+    </row>
+    <row r="625" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D625" s="3"/>
+    </row>
+    <row r="626" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D626" s="3"/>
+    </row>
+    <row r="627" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D627" s="3"/>
+    </row>
+    <row r="628" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D628" s="3"/>
+    </row>
+    <row r="629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D629" s="3"/>
+    </row>
+    <row r="630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D630" s="3"/>
+    </row>
+    <row r="631" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D631" s="3"/>
+    </row>
+    <row r="632" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D632" s="3"/>
+    </row>
+    <row r="633" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D633" s="3"/>
+    </row>
+    <row r="634" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D634" s="3"/>
+    </row>
+    <row r="635" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D635" s="3"/>
+    </row>
+    <row r="636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D636" s="3"/>
+    </row>
+    <row r="637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D637" s="3"/>
+    </row>
+    <row r="638" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D638" s="3"/>
+    </row>
+    <row r="639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D639" s="3"/>
+    </row>
+    <row r="640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D640" s="3"/>
+    </row>
+    <row r="641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D641" s="3"/>
+    </row>
+    <row r="642" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D642" s="3"/>
+    </row>
+    <row r="643" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D643" s="3"/>
+    </row>
+    <row r="644" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D644" s="3"/>
+    </row>
+    <row r="645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D645" s="3"/>
+    </row>
+    <row r="646" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D646" s="3"/>
+    </row>
+    <row r="647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D647" s="3"/>
+    </row>
+    <row r="648" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D648" s="3"/>
+    </row>
+    <row r="649" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D649" s="3"/>
+    </row>
+    <row r="650" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D650" s="3"/>
+    </row>
+    <row r="651" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D651" s="3"/>
+    </row>
+    <row r="652" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D652" s="3"/>
+    </row>
+    <row r="653" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D653" s="3"/>
+    </row>
+    <row r="654" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D654" s="3"/>
+    </row>
+    <row r="655" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D655" s="3"/>
+    </row>
+    <row r="656" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D656" s="3"/>
+    </row>
+    <row r="657" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D657" s="3"/>
+    </row>
+    <row r="658" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D658" s="3"/>
+    </row>
+    <row r="659" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D659" s="3"/>
+    </row>
+    <row r="660" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D660" s="3"/>
+    </row>
+    <row r="661" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D661" s="3"/>
+    </row>
+    <row r="662" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D662" s="3"/>
+    </row>
+    <row r="663" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D663" s="3"/>
+    </row>
+    <row r="664" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D664" s="3"/>
+    </row>
+    <row r="665" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D665" s="3"/>
+    </row>
+    <row r="666" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D666" s="3"/>
+    </row>
+    <row r="667" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D667" s="3"/>
+    </row>
+    <row r="668" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D668" s="3"/>
+    </row>
+    <row r="669" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D669" s="3"/>
+    </row>
+    <row r="670" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D670" s="3"/>
+    </row>
+    <row r="671" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D671" s="3"/>
+    </row>
+    <row r="672" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D672" s="3"/>
+    </row>
+    <row r="673" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D673" s="3"/>
+    </row>
+    <row r="674" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D674" s="3"/>
+    </row>
+    <row r="675" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D675" s="3"/>
+    </row>
+    <row r="676" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D676" s="3"/>
+    </row>
+    <row r="677" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D677" s="3"/>
+    </row>
+    <row r="678" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D678" s="3"/>
+    </row>
+    <row r="679" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D679" s="3"/>
+    </row>
+    <row r="680" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D680" s="3"/>
+    </row>
+    <row r="681" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D681" s="3"/>
+    </row>
+    <row r="682" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D682" s="3"/>
+    </row>
+    <row r="683" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D683" s="3"/>
+    </row>
+    <row r="684" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D684" s="3"/>
+    </row>
+    <row r="685" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D685" s="3"/>
+    </row>
+    <row r="686" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D686" s="3"/>
+    </row>
+    <row r="687" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D687" s="3"/>
+    </row>
+    <row r="688" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D688" s="3"/>
+    </row>
+    <row r="689" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D689" s="3"/>
+    </row>
+    <row r="690" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D690" s="3"/>
+    </row>
+    <row r="691" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D691" s="3"/>
+    </row>
+    <row r="692" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D692" s="3"/>
+    </row>
+    <row r="693" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D693" s="3"/>
+    </row>
+    <row r="694" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D694" s="3"/>
+    </row>
+    <row r="695" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D695" s="3"/>
+    </row>
+    <row r="696" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D696" s="3"/>
+    </row>
+    <row r="697" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D697" s="3"/>
+    </row>
+    <row r="698" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D698" s="3"/>
+    </row>
+    <row r="699" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D699" s="3"/>
+    </row>
+    <row r="700" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D700" s="3"/>
+    </row>
+    <row r="701" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D701" s="3"/>
+    </row>
+    <row r="702" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D702" s="3"/>
+    </row>
+    <row r="703" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D703" s="3"/>
+    </row>
+    <row r="704" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D704" s="3"/>
+    </row>
+    <row r="705" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D705" s="3"/>
+    </row>
+    <row r="706" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D706" s="3"/>
+    </row>
+    <row r="707" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D707" s="3"/>
+    </row>
+    <row r="708" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D708" s="3"/>
+    </row>
+    <row r="709" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D709" s="3"/>
+    </row>
+    <row r="710" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D710" s="3"/>
+    </row>
+    <row r="711" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D711" s="3"/>
+    </row>
+    <row r="712" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D712" s="3"/>
+    </row>
+    <row r="713" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D713" s="3"/>
+    </row>
+    <row r="714" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D714" s="3"/>
+    </row>
+    <row r="715" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D715" s="3"/>
+    </row>
+    <row r="716" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D716" s="3"/>
+    </row>
+    <row r="717" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D717" s="3"/>
+    </row>
+    <row r="718" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D718" s="3"/>
+    </row>
+    <row r="719" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D719" s="3"/>
+    </row>
+    <row r="720" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D720" s="3"/>
+    </row>
+    <row r="721" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D721" s="3"/>
+    </row>
+    <row r="722" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D722" s="3"/>
+    </row>
+    <row r="723" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D723" s="3"/>
+    </row>
+    <row r="724" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D724" s="3"/>
+    </row>
+    <row r="725" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D725" s="3"/>
+    </row>
+    <row r="726" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D726" s="3"/>
+    </row>
+    <row r="727" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D727" s="3"/>
+    </row>
+    <row r="728" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D728" s="3"/>
+    </row>
+    <row r="729" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D729" s="3"/>
+    </row>
+    <row r="730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D730" s="3"/>
+    </row>
+    <row r="731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D731" s="3"/>
+    </row>
+    <row r="732" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D732" s="3"/>
+    </row>
+    <row r="733" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D733" s="3"/>
+    </row>
+    <row r="734" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D734" s="3"/>
+    </row>
+    <row r="735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D735" s="3"/>
+    </row>
+    <row r="736" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D736" s="3"/>
+    </row>
+    <row r="737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D737" s="3"/>
+    </row>
+    <row r="738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D738" s="3"/>
+    </row>
+    <row r="739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D739" s="3"/>
+    </row>
+    <row r="740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D740" s="3"/>
+    </row>
+    <row r="741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D741" s="3"/>
+    </row>
+    <row r="742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D742" s="3"/>
+    </row>
+    <row r="743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D743" s="3"/>
+    </row>
+    <row r="744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D744" s="3"/>
+    </row>
+    <row r="745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D745" s="3"/>
+    </row>
+    <row r="746" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D746" s="3"/>
+    </row>
+    <row r="747" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D747" s="3"/>
+    </row>
+    <row r="748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D748" s="3"/>
+    </row>
+    <row r="749" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D749" s="3"/>
+    </row>
+    <row r="750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D750" s="3"/>
+    </row>
+    <row r="751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D751" s="3"/>
+    </row>
+    <row r="752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D752" s="3"/>
+    </row>
+    <row r="753" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D753" s="3"/>
+    </row>
+    <row r="754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D754" s="3"/>
+    </row>
+    <row r="755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D755" s="3"/>
+    </row>
+    <row r="756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D756" s="3"/>
+    </row>
+    <row r="757" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D757" s="3"/>
+    </row>
+    <row r="758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D758" s="3"/>
+    </row>
+    <row r="759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D759" s="3"/>
+    </row>
+    <row r="760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D760" s="3"/>
+    </row>
+    <row r="761" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D761" s="3"/>
+    </row>
+    <row r="762" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D762" s="3"/>
+    </row>
+    <row r="763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D763" s="3"/>
+    </row>
+    <row r="764" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D764" s="3"/>
+    </row>
+    <row r="765" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D765" s="3"/>
+    </row>
+    <row r="766" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D766" s="3"/>
+    </row>
+    <row r="767" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D767" s="3"/>
+    </row>
+    <row r="768" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D768" s="3"/>
+    </row>
+    <row r="769" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D769" s="3"/>
+    </row>
+    <row r="770" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D770" s="3"/>
+    </row>
+    <row r="771" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D771" s="3"/>
+    </row>
+    <row r="772" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D772" s="3"/>
+    </row>
+    <row r="773" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D773" s="3"/>
+    </row>
+    <row r="774" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D774" s="3"/>
+    </row>
+    <row r="775" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D775" s="3"/>
+    </row>
+    <row r="776" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D776" s="3"/>
+    </row>
+    <row r="777" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D777" s="3"/>
+    </row>
+    <row r="778" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D778" s="3"/>
+    </row>
+    <row r="779" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D779" s="3"/>
+    </row>
+    <row r="780" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D780" s="3"/>
+    </row>
+    <row r="781" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D781" s="3"/>
+    </row>
+    <row r="782" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D782" s="3"/>
+    </row>
+    <row r="783" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D783" s="3"/>
+    </row>
+    <row r="784" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D784" s="3"/>
+    </row>
+    <row r="785" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D785" s="3"/>
+    </row>
+    <row r="786" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D786" s="3"/>
+    </row>
+    <row r="787" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D787" s="3"/>
+    </row>
+    <row r="788" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D788" s="3"/>
+    </row>
+    <row r="789" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D789" s="3"/>
+    </row>
+    <row r="790" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D790" s="3"/>
+    </row>
+    <row r="791" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D791" s="3"/>
+    </row>
+    <row r="792" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D792" s="3"/>
+    </row>
+    <row r="793" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D793" s="3"/>
+    </row>
+    <row r="794" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D794" s="3"/>
+    </row>
+    <row r="795" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D795" s="3"/>
+    </row>
+    <row r="796" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D796" s="3"/>
+    </row>
+    <row r="797" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D797" s="3"/>
+    </row>
+    <row r="798" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D798" s="3"/>
+    </row>
+    <row r="799" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D799" s="3"/>
+    </row>
+    <row r="800" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D800" s="3"/>
+    </row>
+    <row r="801" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D801" s="3"/>
+    </row>
+    <row r="802" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D802" s="3"/>
+    </row>
+    <row r="803" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D803" s="3"/>
+    </row>
+    <row r="804" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D804" s="3"/>
+    </row>
+    <row r="805" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D805" s="3"/>
+    </row>
+    <row r="806" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D806" s="3"/>
+    </row>
+    <row r="807" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D807" s="3"/>
+    </row>
+    <row r="808" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D808" s="3"/>
+    </row>
+    <row r="809" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D809" s="3"/>
+    </row>
+    <row r="810" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D810" s="3"/>
+    </row>
+    <row r="811" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D811" s="3"/>
+    </row>
+    <row r="812" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D812" s="3"/>
+    </row>
+    <row r="813" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D813" s="3"/>
+    </row>
+    <row r="814" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D814" s="3"/>
+    </row>
+    <row r="815" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D815" s="3"/>
+    </row>
+    <row r="816" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D816" s="3"/>
+    </row>
+    <row r="817" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D817" s="3"/>
+    </row>
+    <row r="818" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D818" s="3"/>
+    </row>
+    <row r="819" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D819" s="3"/>
+    </row>
+    <row r="820" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D820" s="3"/>
+    </row>
+    <row r="821" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D821" s="3"/>
+    </row>
+    <row r="822" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D822" s="3"/>
+    </row>
+    <row r="823" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D823" s="3"/>
+    </row>
+    <row r="824" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D824" s="3"/>
+    </row>
+    <row r="825" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D825" s="3"/>
+    </row>
+    <row r="826" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D826" s="3"/>
+    </row>
+    <row r="827" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D827" s="3"/>
+    </row>
+    <row r="828" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D828" s="3"/>
+    </row>
+    <row r="829" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D829" s="3"/>
+    </row>
+    <row r="830" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D830" s="3"/>
+    </row>
+    <row r="831" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D831" s="3"/>
+    </row>
+    <row r="832" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D832" s="3"/>
+    </row>
+    <row r="833" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D833" s="3"/>
+    </row>
+    <row r="834" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D834" s="3"/>
+    </row>
+    <row r="835" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D835" s="3"/>
+    </row>
+    <row r="836" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D836" s="3"/>
+    </row>
+    <row r="837" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D837" s="3"/>
+    </row>
+    <row r="838" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D838" s="3"/>
+    </row>
+    <row r="839" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D839" s="3"/>
+    </row>
+    <row r="840" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D840" s="3"/>
+    </row>
+    <row r="841" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D841" s="3"/>
+    </row>
+    <row r="842" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D842" s="3"/>
+    </row>
+    <row r="843" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D843" s="3"/>
+    </row>
+    <row r="844" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D844" s="3"/>
+    </row>
+    <row r="845" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D845" s="3"/>
+    </row>
+    <row r="846" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D846" s="3"/>
+    </row>
+    <row r="847" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D847" s="3"/>
+    </row>
+    <row r="848" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D848" s="3"/>
+    </row>
+    <row r="849" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D849" s="3"/>
+    </row>
+    <row r="850" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D850" s="3"/>
+    </row>
+    <row r="851" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D851" s="3"/>
+    </row>
+    <row r="852" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D852" s="3"/>
+    </row>
+    <row r="853" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D853" s="3"/>
+    </row>
+    <row r="854" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D854" s="3"/>
+    </row>
+    <row r="855" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D855" s="3"/>
+    </row>
+    <row r="856" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D856" s="3"/>
+    </row>
+    <row r="857" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D857" s="3"/>
+    </row>
+    <row r="858" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D858" s="3"/>
+    </row>
+    <row r="859" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D859" s="3"/>
+    </row>
+    <row r="860" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D860" s="3"/>
+    </row>
+    <row r="861" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D861" s="3"/>
+    </row>
+    <row r="862" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D862" s="3"/>
+    </row>
+    <row r="863" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D863" s="3"/>
+    </row>
+    <row r="864" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D864" s="3"/>
+    </row>
+    <row r="865" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D865" s="3"/>
+    </row>
+    <row r="866" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D866" s="3"/>
+    </row>
+    <row r="867" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D867" s="3"/>
+    </row>
+    <row r="868" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D868" s="3"/>
+    </row>
+    <row r="869" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D869" s="3"/>
+    </row>
+    <row r="870" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D870" s="3"/>
+    </row>
+    <row r="871" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D871" s="3"/>
+    </row>
+    <row r="872" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D872" s="3"/>
+    </row>
+    <row r="873" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D873" s="3"/>
+    </row>
+    <row r="874" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D874" s="3"/>
+    </row>
+    <row r="875" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D875" s="3"/>
+    </row>
+    <row r="876" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D876" s="3"/>
+    </row>
+    <row r="877" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D877" s="3"/>
+    </row>
+    <row r="878" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D878" s="3"/>
+    </row>
+    <row r="879" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D879" s="3"/>
+    </row>
+    <row r="880" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D880" s="3"/>
+    </row>
+    <row r="881" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D881" s="3"/>
+    </row>
+    <row r="882" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D882" s="3"/>
+    </row>
+    <row r="883" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D883" s="3"/>
+    </row>
+    <row r="884" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D884" s="3"/>
+    </row>
+    <row r="885" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D885" s="3"/>
+    </row>
+    <row r="886" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D886" s="3"/>
+    </row>
+    <row r="887" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D887" s="3"/>
+    </row>
+    <row r="888" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D888" s="3"/>
+    </row>
+    <row r="889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D889" s="3"/>
+    </row>
+    <row r="890" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D890" s="3"/>
+    </row>
+    <row r="891" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D891" s="3"/>
+    </row>
+    <row r="892" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D892" s="3"/>
+    </row>
+    <row r="893" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D893" s="3"/>
+    </row>
+    <row r="894" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D894" s="3"/>
+    </row>
+    <row r="895" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D895" s="3"/>
+    </row>
+    <row r="896" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D896" s="3"/>
+    </row>
+    <row r="897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D897" s="3"/>
+    </row>
+    <row r="898" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D898" s="3"/>
+    </row>
+    <row r="899" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D899" s="3"/>
+    </row>
+    <row r="900" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D900" s="3"/>
+    </row>
+    <row r="901" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D901" s="3"/>
+    </row>
+    <row r="902" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D902" s="3"/>
+    </row>
+    <row r="903" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D903" s="3"/>
+    </row>
+    <row r="904" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D904" s="3"/>
+    </row>
+    <row r="905" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D905" s="3"/>
+    </row>
+    <row r="906" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D906" s="3"/>
+    </row>
+    <row r="907" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D907" s="3"/>
+    </row>
+    <row r="908" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D908" s="3"/>
+    </row>
+    <row r="909" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D909" s="3"/>
+    </row>
+    <row r="910" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D910" s="3"/>
+    </row>
+    <row r="911" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D911" s="3"/>
+    </row>
+    <row r="912" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D912" s="3"/>
+    </row>
+    <row r="913" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D913" s="3"/>
+    </row>
+    <row r="914" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D914" s="3"/>
+    </row>
+    <row r="915" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D915" s="3"/>
+    </row>
+    <row r="916" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D916" s="3"/>
+    </row>
+    <row r="917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D917" s="3"/>
+    </row>
+    <row r="918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D918" s="3"/>
+    </row>
+    <row r="919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D919" s="3"/>
+    </row>
+    <row r="920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D920" s="3"/>
+    </row>
+    <row r="921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D921" s="3"/>
+    </row>
+    <row r="922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D922" s="3"/>
+    </row>
+    <row r="923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D923" s="3"/>
+    </row>
+    <row r="924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D924" s="3"/>
+    </row>
+    <row r="925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D925" s="3"/>
+    </row>
+    <row r="926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D926" s="3"/>
+    </row>
+    <row r="927" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D927" s="3"/>
+    </row>
+    <row r="928" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D928" s="3"/>
+    </row>
+    <row r="929" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D929" s="3"/>
+    </row>
+    <row r="930" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D930" s="3"/>
+    </row>
+    <row r="931" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D931" s="3"/>
+    </row>
+    <row r="932" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D932" s="3"/>
+    </row>
+    <row r="933" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D933" s="3"/>
+    </row>
+    <row r="934" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D934" s="3"/>
+    </row>
+    <row r="935" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D935" s="3"/>
+    </row>
+    <row r="936" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D936" s="3"/>
+    </row>
+    <row r="937" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D937" s="3"/>
+    </row>
+    <row r="938" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D938" s="3"/>
+    </row>
+    <row r="939" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D939" s="3"/>
+    </row>
+    <row r="940" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D940" s="3"/>
+    </row>
+    <row r="941" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D941" s="3"/>
+    </row>
+    <row r="942" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D942" s="3"/>
+    </row>
+    <row r="943" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D943" s="3"/>
+    </row>
+    <row r="944" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D944" s="3"/>
+    </row>
+    <row r="945" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D945" s="3"/>
+    </row>
+    <row r="946" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D946" s="3"/>
+    </row>
+    <row r="947" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D947" s="3"/>
+    </row>
+    <row r="948" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D948" s="3"/>
+    </row>
+    <row r="949" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D949" s="3"/>
+    </row>
+    <row r="950" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D950" s="3"/>
+    </row>
+    <row r="951" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D951" s="3"/>
+    </row>
+    <row r="952" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D952" s="3"/>
+    </row>
+    <row r="953" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D953" s="3"/>
+    </row>
+    <row r="954" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D954" s="3"/>
+    </row>
+    <row r="955" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D955" s="3"/>
+    </row>
+    <row r="956" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D956" s="3"/>
+    </row>
+    <row r="957" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D957" s="3"/>
+    </row>
+    <row r="958" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D958" s="3"/>
+    </row>
+    <row r="959" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D959" s="3"/>
+    </row>
+    <row r="960" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D960" s="3"/>
+    </row>
+    <row r="961" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D961" s="3"/>
+    </row>
+    <row r="962" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D962" s="3"/>
+    </row>
+    <row r="963" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D963" s="3"/>
+    </row>
+    <row r="964" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D964" s="3"/>
+    </row>
+    <row r="965" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D965" s="3"/>
+    </row>
+    <row r="966" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D966" s="3"/>
+    </row>
+    <row r="967" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D967" s="3"/>
+    </row>
+    <row r="968" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D968" s="3"/>
+    </row>
+    <row r="969" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D969" s="3"/>
+    </row>
+    <row r="970" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D970" s="3"/>
+    </row>
+    <row r="971" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D971" s="3"/>
+    </row>
+    <row r="972" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D972" s="3"/>
+    </row>
+    <row r="973" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D973" s="3"/>
+    </row>
+    <row r="974" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D974" s="3"/>
+    </row>
+    <row r="975" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D975" s="3"/>
+    </row>
+    <row r="976" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D976" s="3"/>
+    </row>
+    <row r="977" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D977" s="3"/>
+    </row>
+    <row r="978" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D978" s="3"/>
+    </row>
+    <row r="979" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D979" s="3"/>
+    </row>
+    <row r="980" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D980" s="3"/>
+    </row>
+    <row r="981" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D981" s="3"/>
+    </row>
+    <row r="982" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D982" s="3"/>
+    </row>
+    <row r="983" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D983" s="3"/>
+    </row>
+    <row r="984" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D984" s="3"/>
+    </row>
+    <row r="985" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D985" s="3"/>
+    </row>
+    <row r="986" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D986" s="3"/>
+    </row>
+    <row r="987" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D987" s="3"/>
+    </row>
+    <row r="988" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D988" s="3"/>
+    </row>
+    <row r="989" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D989" s="3"/>
+    </row>
+    <row r="990" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D990" s="3"/>
+    </row>
+    <row r="991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D991" s="3"/>
+    </row>
+    <row r="992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D992" s="3"/>
+    </row>
+    <row r="993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D993" s="3"/>
+    </row>
+    <row r="994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D994" s="3"/>
+    </row>
+    <row r="995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D995" s="3"/>
+    </row>
+    <row r="996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D996" s="3"/>
+    </row>
+    <row r="997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D997" s="3"/>
+    </row>
+    <row r="998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D998" s="3"/>
+    </row>
+    <row r="999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D999" s="3"/>
+    </row>
+    <row r="1000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1000" s="3"/>
+    </row>
+    <row r="1001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1001" s="3"/>
+    </row>
+    <row r="1002" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1002" s="3"/>
+    </row>
+    <row r="1003" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1003" s="3"/>
+    </row>
+    <row r="1004" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1004" s="3"/>
+    </row>
+    <row r="1005" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1005" s="3"/>
+    </row>
+    <row r="1006" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1006" s="3"/>
+    </row>
+    <row r="1007" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1007" s="3"/>
+    </row>
+    <row r="1008" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1008" s="3"/>
+    </row>
+    <row r="1009" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1009" s="3"/>
+    </row>
+    <row r="1010" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1010" s="3"/>
+    </row>
+    <row r="1011" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1011" s="3"/>
+    </row>
+    <row r="1012" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1012" s="3"/>
+    </row>
+    <row r="1013" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1013" s="3"/>
+    </row>
+    <row r="1014" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1014" s="3"/>
+    </row>
+    <row r="1015" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1015" s="3"/>
+    </row>
+    <row r="1016" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1016" s="3"/>
+    </row>
+    <row r="1017" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1017" s="3"/>
+    </row>
+    <row r="1018" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1018" s="3"/>
+    </row>
+    <row r="1019" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1019" s="3"/>
+    </row>
+    <row r="1020" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1020" s="3"/>
+    </row>
+    <row r="1021" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1021" s="3"/>
+    </row>
+    <row r="1022" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1022" s="3"/>
+    </row>
+    <row r="1023" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1023" s="3"/>
+    </row>
+    <row r="1024" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1024" s="3"/>
+    </row>
+    <row r="1025" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1025" s="3"/>
+    </row>
+    <row r="1026" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1026" s="3"/>
+    </row>
+    <row r="1027" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1027" s="3"/>
+    </row>
+    <row r="1028" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1028" s="3"/>
+    </row>
+    <row r="1029" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1029" s="3"/>
+    </row>
+    <row r="1030" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1030" s="3"/>
+    </row>
+    <row r="1031" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1031" s="3"/>
+    </row>
+    <row r="1032" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1032" s="3"/>
+    </row>
+    <row r="1033" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1033" s="3"/>
+    </row>
+    <row r="1034" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1034" s="3"/>
+    </row>
+    <row r="1035" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1035" s="3"/>
+    </row>
+    <row r="1036" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1036" s="3"/>
+    </row>
+    <row r="1037" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1037" s="3"/>
+    </row>
+    <row r="1038" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1038" s="3"/>
+    </row>
+    <row r="1039" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1039" s="3"/>
+    </row>
+    <row r="1040" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1040" s="3"/>
+    </row>
+    <row r="1041" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1041" s="3"/>
+    </row>
+    <row r="1042" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1042" s="3"/>
+    </row>
+    <row r="1043" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1043" s="3"/>
+    </row>
+    <row r="1044" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1044" s="3"/>
+    </row>
+    <row r="1045" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1045" s="3"/>
+    </row>
+    <row r="1046" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1046" s="3"/>
+    </row>
+    <row r="1047" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1047" s="3"/>
+    </row>
+    <row r="1048" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1048" s="3"/>
+    </row>
+    <row r="1049" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1049" s="3"/>
+    </row>
+    <row r="1050" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1050" s="3"/>
+    </row>
+    <row r="1051" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1051" s="3"/>
+    </row>
+    <row r="1052" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1052" s="3"/>
+    </row>
+    <row r="1053" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1053" s="3"/>
+    </row>
+    <row r="1054" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1054" s="3"/>
+    </row>
+    <row r="1055" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1055" s="3"/>
+    </row>
+    <row r="1056" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1056" s="3"/>
+    </row>
+    <row r="1057" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1057" s="3"/>
+    </row>
+    <row r="1058" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1058" s="3"/>
+    </row>
+    <row r="1059" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1059" s="3"/>
+    </row>
+    <row r="1060" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1060" s="3"/>
+    </row>
+    <row r="1061" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1061" s="3"/>
+    </row>
+    <row r="1062" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1062" s="3"/>
+    </row>
+    <row r="1063" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1063" s="3"/>
+    </row>
+    <row r="1064" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1064" s="3"/>
+    </row>
+    <row r="1065" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1065" s="3"/>
+    </row>
+    <row r="1066" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1066" s="3"/>
+    </row>
+    <row r="1067" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1067" s="3"/>
+    </row>
+    <row r="1068" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1068" s="3"/>
+    </row>
+    <row r="1069" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1069" s="3"/>
+    </row>
+    <row r="1070" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1070" s="3"/>
+    </row>
+    <row r="1071" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1071" s="3"/>
+    </row>
+    <row r="1072" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1072" s="3"/>
+    </row>
+    <row r="1073" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1073" s="3"/>
+    </row>
+    <row r="1074" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1074" s="3"/>
+    </row>
+    <row r="1075" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1075" s="3"/>
+    </row>
+    <row r="1076" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1076" s="3"/>
+    </row>
+    <row r="1077" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1077" s="3"/>
+    </row>
+    <row r="1078" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1078" s="3"/>
+    </row>
+    <row r="1079" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1079" s="3"/>
+    </row>
+    <row r="1080" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1080" s="3"/>
+    </row>
+    <row r="1081" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1081" s="3"/>
+    </row>
+    <row r="1082" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1082" s="3"/>
+    </row>
+    <row r="1083" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1083" s="3"/>
+    </row>
+    <row r="1084" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1084" s="3"/>
+    </row>
+    <row r="1085" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1085" s="3"/>
+    </row>
+    <row r="1086" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1086" s="3"/>
+    </row>
+    <row r="1087" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1087" s="3"/>
+    </row>
+    <row r="1088" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1088" s="3"/>
+    </row>
+    <row r="1089" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1089" s="3"/>
+    </row>
+    <row r="1090" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1090" s="3"/>
+    </row>
+    <row r="1091" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1091" s="3"/>
+    </row>
+    <row r="1092" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1092" s="3"/>
+    </row>
+    <row r="1093" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1093" s="3"/>
+    </row>
+    <row r="1094" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1094" s="3"/>
+    </row>
+    <row r="1095" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1095" s="3"/>
+    </row>
+    <row r="1096" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1096" s="3"/>
+    </row>
+    <row r="1097" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1097" s="3"/>
+    </row>
+    <row r="1098" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1098" s="3"/>
+    </row>
+    <row r="1099" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1099" s="3"/>
+    </row>
+    <row r="1100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1100" s="3"/>
+    </row>
+    <row r="1101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1101" s="3"/>
+    </row>
+    <row r="1102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1102" s="3"/>
+    </row>
+    <row r="1103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1103" s="3"/>
+    </row>
+    <row r="1104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1104" s="3"/>
+    </row>
+    <row r="1105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1105" s="3"/>
+    </row>
+    <row r="1106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1106" s="3"/>
+    </row>
+    <row r="1107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1107" s="3"/>
+    </row>
+    <row r="1108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1108" s="3"/>
+    </row>
+    <row r="1109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1109" s="3"/>
+    </row>
+    <row r="1110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1110" s="3"/>
+    </row>
+    <row r="1111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1111" s="3"/>
+    </row>
+    <row r="1112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1112" s="3"/>
+    </row>
+    <row r="1113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1113" s="3"/>
+    </row>
+    <row r="1114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1114" s="3"/>
+    </row>
+    <row r="1115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1115" s="3"/>
+    </row>
+    <row r="1116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1116" s="3"/>
+    </row>
+    <row r="1117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1117" s="3"/>
+    </row>
+    <row r="1118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1118" s="3"/>
+    </row>
+    <row r="1119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1119" s="3"/>
+    </row>
+    <row r="1120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1120" s="3"/>
+    </row>
+    <row r="1121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1121" s="3"/>
+    </row>
+    <row r="1122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1122" s="3"/>
+    </row>
+    <row r="1123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1123" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>